<commit_message>
WG N numbers table template
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_210_2/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_210_2/WG_Number_excel_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klt/Projets/EclipseWS/stepmod/publication/part1000/CR_210_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klt/Projets/EclipseWS/stepmod/publication/part1000/CR_210_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Submitter</t>
+  </si>
+  <si>
+    <t>request date</t>
+  </si>
+  <si>
+    <t>Document and schema</t>
+  </si>
+  <si>
+    <t>N#</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -391,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -404,12 +417,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>

</xml_diff>

<commit_message>
moved 410 from CR_210_2 to CR_designAPs_1, updated WG N nb table, committed build files
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_210_2/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_210_2/WG_Number_excel_table.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
   <si>
     <t>Submitter</t>
   </si>
@@ -38,15 +38,6 @@
     <t>N#</t>
   </si>
   <si>
-    <t>ISO 10303-410 ed4 ap210_electronic_assembly_interconnect_and_packaging_design Document</t>
-  </si>
-  <si>
-    <t>ISO 10303-410 ed4 ap210_electronic_assembly_interconnect_and_packaging_design ARM EXPRESS</t>
-  </si>
-  <si>
-    <t>ISO 10303-410 ed4 ap210_electronic_assembly_interconnect_and_packaging_design MIM EXPRESS</t>
-  </si>
-  <si>
     <t>ISO 10303-1404 ed2 geometric_model_2d_3d_relationship Document</t>
   </si>
   <si>
@@ -81,15 +72,6 @@
   </si>
   <si>
     <t>Aminata Mbengue</t>
-  </si>
-  <si>
-    <t>N9374</t>
-  </si>
-  <si>
-    <t>N9375</t>
-  </si>
-  <si>
-    <t>N9376</t>
   </si>
   <si>
     <t>N9377</t>
@@ -681,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -705,7 +687,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -719,10 +701,10 @@
     </row>
     <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -730,7 +712,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -742,10 +724,10 @@
     </row>
     <row r="3" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -753,7 +735,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -765,18 +747,18 @@
     </row>
     <row r="4" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="9" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -788,18 +770,18 @@
     </row>
     <row r="5" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="9" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -811,18 +793,18 @@
     </row>
     <row r="6" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -834,18 +816,18 @@
     </row>
     <row r="7" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="9" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -857,18 +839,18 @@
     </row>
     <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="9" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -878,66 +860,54 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="9" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="9" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="9" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -947,54 +917,66 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="9" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -1006,18 +988,18 @@
     </row>
     <row r="15" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="9" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -1029,18 +1011,18 @@
     </row>
     <row r="16" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="9" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -1052,18 +1034,18 @@
     </row>
     <row r="17" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="9" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1075,18 +1057,18 @@
     </row>
     <row r="18" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="9" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1098,18 +1080,18 @@
     </row>
     <row r="19" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="9" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1121,18 +1103,18 @@
     </row>
     <row r="20" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="9" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -1144,18 +1126,18 @@
     </row>
     <row r="21" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="9" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -1165,20 +1147,20 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="9" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -1188,20 +1170,20 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -1213,18 +1195,18 @@
     </row>
     <row r="24" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="9" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -1234,20 +1216,20 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="9" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -1257,20 +1239,20 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="9" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -1282,10 +1264,10 @@
     </row>
     <row r="27" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1293,7 +1275,7 @@
         <v>11</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -1303,20 +1285,20 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="9" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -1326,20 +1308,20 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -1351,18 +1333,18 @@
     </row>
     <row r="30" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="9" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -1372,20 +1354,20 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="9" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -1395,20 +1377,20 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -1420,18 +1402,18 @@
     </row>
     <row r="33" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="9" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -1443,100 +1425,31 @@
     </row>
     <row r="34" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="9" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="35" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-    </row>
-    <row r="37" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-    </row>
-    <row r="39" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>